<commit_message>
added new TP excel files, added new conditions file and generated mat, removed debug values
</commit_message>
<xml_diff>
--- a/xls/correct/G1_TP_A.xlsx
+++ b/xls/correct/G1_TP_A.xlsx
@@ -16,15 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="20">
   <si>
     <t>pe</t>
   </si>
   <si>
     <t>lo</t>
-  </si>
-  <si>
-    <t>ta</t>
   </si>
   <si>
     <t>fu</t>
@@ -57,28 +54,28 @@
     <t>mi</t>
   </si>
   <si>
-    <t>la</t>
-  </si>
-  <si>
-    <t>ra</t>
-  </si>
-  <si>
     <t>po</t>
-  </si>
-  <si>
-    <t>so</t>
-  </si>
-  <si>
-    <t>bo</t>
-  </si>
-  <si>
-    <t>wa</t>
   </si>
   <si>
     <t>do</t>
   </si>
   <si>
     <t>fe</t>
+  </si>
+  <si>
+    <t>li</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>sa</t>
   </si>
 </sst>
 </file>
@@ -419,15 +416,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R69" sqref="R69"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -436,16 +433,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1">
         <v>11</v>
@@ -468,25 +465,25 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>11</v>
@@ -509,25 +506,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <v>11</v>
@@ -550,25 +547,25 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>11</v>
@@ -591,25 +588,25 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <v>11</v>
@@ -632,25 +629,25 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <v>11</v>
@@ -673,25 +670,25 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <v>11</v>
@@ -714,25 +711,25 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <v>11</v>
@@ -755,25 +752,25 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H9">
         <v>11</v>
@@ -796,25 +793,25 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10">
         <v>11</v>
@@ -837,25 +834,25 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>11</v>
@@ -878,25 +875,25 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <v>11</v>
@@ -919,10 +916,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -931,13 +928,13 @@
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <v>11</v>
@@ -960,25 +957,25 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H14">
         <v>11</v>
@@ -1001,25 +998,25 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H15">
         <v>11</v>
@@ -1042,25 +1039,25 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16">
         <v>11</v>
@@ -1083,25 +1080,25 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H17">
         <v>11</v>
@@ -1124,25 +1121,25 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <v>11</v>
@@ -1165,25 +1162,25 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <v>11</v>
@@ -1206,25 +1203,25 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H20">
         <v>11</v>
@@ -1247,25 +1244,25 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <v>11</v>
@@ -1288,25 +1285,25 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <v>11</v>
@@ -1329,7 +1326,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1338,16 +1335,16 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H23">
         <v>11</v>
@@ -1370,25 +1367,25 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H24">
         <v>11</v>
@@ -1411,25 +1408,25 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H25">
         <v>11</v>
@@ -1452,25 +1449,25 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26">
         <v>11</v>
@@ -1493,25 +1490,25 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H27">
         <v>11</v>
@@ -1534,25 +1531,25 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G28" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H28">
         <v>11</v>
@@ -1575,25 +1572,25 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H29">
         <v>11</v>
@@ -1616,25 +1613,25 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <v>11</v>
@@ -1657,25 +1654,25 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H31">
         <v>11</v>
@@ -1698,25 +1695,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>17</v>
-      </c>
       <c r="E32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H32">
         <v>11</v>
@@ -1739,25 +1736,25 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H33">
         <v>11</v>
@@ -1780,25 +1777,25 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H34">
         <v>11</v>
@@ -1821,25 +1818,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H35">
         <v>11</v>
@@ -1862,25 +1859,25 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H36">
         <v>11</v>
@@ -1903,25 +1900,25 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H37">
         <v>11</v>
@@ -1944,25 +1941,25 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H38">
         <v>11</v>
@@ -1985,25 +1982,25 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H39">
         <v>11</v>
@@ -2026,25 +2023,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H40">
         <v>11</v>
@@ -2067,25 +2064,25 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G41" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H41">
         <v>11</v>
@@ -2108,7 +2105,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
@@ -2117,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H42">
         <v>11</v>
@@ -2149,25 +2146,25 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
         <v>18</v>
       </c>
-      <c r="B43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s">
-        <v>15</v>
-      </c>
       <c r="E43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H43">
         <v>11</v>
@@ -2190,7 +2187,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
@@ -2199,16 +2196,16 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H44">
         <v>11</v>
@@ -2231,25 +2228,25 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H45">
         <v>11</v>
@@ -2272,25 +2269,25 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H46">
         <v>11</v>
@@ -2313,25 +2310,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H47">
         <v>11</v>
@@ -2354,25 +2351,25 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
         <v>6</v>
       </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" t="s">
-        <v>10</v>
-      </c>
       <c r="E48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G48" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H48">
         <v>11</v>
@@ -2395,25 +2392,25 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H49">
         <v>11</v>
@@ -2436,25 +2433,25 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G50" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H50">
         <v>11</v>
@@ -2477,7 +2474,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
         <v>0</v>
@@ -2486,16 +2483,16 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H51">
         <v>11</v>
@@ -2518,25 +2515,25 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H52">
         <v>11</v>
@@ -2559,7 +2556,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B53" t="s">
         <v>0</v>
@@ -2568,16 +2565,16 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H53">
         <v>11</v>
@@ -2600,25 +2597,25 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
         <v>6</v>
       </c>
-      <c r="C54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>12</v>
-      </c>
       <c r="E54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H54">
         <v>11</v>
@@ -2641,25 +2638,25 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D55" t="s">
         <v>15</v>
       </c>
       <c r="E55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H55">
         <v>11</v>
@@ -2682,25 +2679,25 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G56" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H56">
         <v>11</v>
@@ -2723,25 +2720,25 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G57" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H57">
         <v>11</v>
@@ -2764,25 +2761,25 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B58" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G58" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H58">
         <v>11</v>
@@ -2805,25 +2802,25 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H59">
         <v>11</v>
@@ -2846,25 +2843,25 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G60" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H60">
         <v>11</v>
@@ -2887,7 +2884,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
         <v>0</v>
@@ -2896,16 +2893,16 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H61">
         <v>11</v>
@@ -2928,25 +2925,25 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H62">
         <v>11</v>
@@ -2969,25 +2966,25 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D63" t="s">
         <v>10</v>
       </c>
       <c r="E63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H63">
         <v>11</v>
@@ -3010,25 +3007,25 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
         <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G64" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H64">
         <v>11</v>

</xml_diff>